<commit_message>
edits to the reports
</commit_message>
<xml_diff>
--- a/T3-Reports/T3_status_091020.xlsx
+++ b/T3-Reports/T3_status_091020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeenatbaig/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeenatbaig/Documents/GitHub/order-book-project-team-3/T3-Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A48B5BE-3B26-374F-95CC-809E91E3814B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9FC03C-FCD5-B143-A585-9C2692DAA208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="3980" windowWidth="23960" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="540" windowWidth="23960" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Report" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Project</t>
   </si>
@@ -161,9 +161,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Status Report for Team Bubbles - Class Project</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zeenat </t>
   </si>
   <si>
@@ -173,21 +170,9 @@
     <t>Working through main ideas of project.</t>
   </si>
   <si>
-    <t>Buchi</t>
-  </si>
-  <si>
-    <t>Anmol</t>
-  </si>
-  <si>
     <t>Eric</t>
   </si>
   <si>
-    <t xml:space="preserve">Lead </t>
-  </si>
-  <si>
-    <t>reviewed aspects of order books</t>
-  </si>
-  <si>
     <t>out sick</t>
   </si>
   <si>
@@ -207,6 +192,24 @@
   </si>
   <si>
     <t xml:space="preserve">waiting on answer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reviewed aspects of order books and went over more requirements for the project </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reviewed aspects of order books and went over more requirements for the project </t>
+  </si>
+  <si>
+    <t>Status Report for Team 3 - Orderbook  Project</t>
+  </si>
+  <si>
+    <t>Zeenat (Lead)</t>
+  </si>
+  <si>
+    <t>Buchi (frontend)</t>
+  </si>
+  <si>
+    <t>Anmol(backend)</t>
   </si>
 </sst>
 </file>
@@ -515,6 +518,12 @@
     <xf numFmtId="16" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -523,12 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -910,7 +913,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -922,15 +925,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -963,8 +966,8 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="33" t="s">
-        <v>27</v>
+      <c r="E4" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -974,28 +977,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="E5" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
@@ -1029,10 +1032,10 @@
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -1042,10 +1045,10 @@
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1055,10 +1058,10 @@
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1068,10 +1071,10 @@
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1110,11 +1113,11 @@
         <v>1</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -1194,8 +1197,8 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
-      <c r="D23" s="34" t="s">
-        <v>37</v>
+      <c r="D23" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="14"/>
@@ -1207,8 +1210,8 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="34" t="s">
-        <v>37</v>
+      <c r="D24" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="14"/>
@@ -1220,8 +1223,8 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
-      <c r="D25" s="34" t="s">
-        <v>37</v>
+      <c r="D25" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="14"/>
@@ -1233,8 +1236,8 @@
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
-      <c r="D26" s="34" t="s">
-        <v>37</v>
+      <c r="D26" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="14"/>
@@ -1246,8 +1249,8 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="34" t="s">
-        <v>37</v>
+      <c r="D27" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="14"/>
@@ -1255,16 +1258,16 @@
     </row>
     <row r="28" spans="1:7" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G28" s="15"/>
     </row>

</xml_diff>